<commit_message>
Added all template .tex files, changed the name and ordering of sections, reached Write Away 10
</commit_message>
<xml_diff>
--- a/LightSpan Adventure List of Games.xlsx
+++ b/LightSpan Adventure List of Games.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Defined list of the games"/>
@@ -1152,7 +1152,7 @@
   </sheetPr>
   <dimension ref="A1:A992"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1484,172 +1484,172 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A66" s="8" t="s">
         <v>172</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A67" s="8" t="s">
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A68" s="8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A69" s="8" t="s">
         <v>175</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A70" s="8" t="s">
         <v>176</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A71" s="8" t="s">
         <v>177</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A72" s="8" t="s">
         <v>178</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A73" s="8" t="s">
         <v>179</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A74" s="8" t="s">
         <v>180</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A75" s="8" t="s">
         <v>181</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A76" s="8" t="s">
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A77" s="8" t="s">
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A78" s="8" t="s">
         <v>184</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A79" s="8" t="s">
         <v>185</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A80" s="8" t="s">
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A81" s="8" t="s">
         <v>187</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A82" s="8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A83" s="8" t="s">
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A84" s="8" t="s">
         <v>190</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A85" s="8" t="s">
         <v>191</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A86" s="8" t="s">
         <v>192</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A87" s="8" t="s">
         <v>193</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A88" s="8" t="s">
         <v>194</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A89" s="8" t="s">
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A90" s="8" t="s">
         <v>196</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A91" s="8" t="s">
         <v>197</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A92" s="8" t="s">
         <v>198</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A93" s="8" t="s">
         <v>199</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A94" s="8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A95" s="8" t="s">
         <v>201</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A96" s="8" t="s">
         <v>202</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A97" s="8" t="s">
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A98" s="8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="15.75" customFormat="1" s="7">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" customFormat="1" s="7">
       <c r="A99" s="8" t="s">
         <v>205</v>
       </c>
@@ -4384,7 +4384,7 @@
   </sheetPr>
   <dimension ref="A1:J999"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>